<commit_message>
Tratamento inicial de dados
</commit_message>
<xml_diff>
--- a/Tratamento de Dados.xlsx
+++ b/Tratamento de Dados.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
+    <sheet name="Colunas e Relação com Vazio" sheetId="1" r:id="rId1"/>
+    <sheet name="Linhas com Satisfação 99" sheetId="3" r:id="rId2"/>
+    <sheet name="Plan2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="137">
   <si>
     <t>IDTNS</t>
   </si>
@@ -433,6 +434,9 @@
   </si>
   <si>
     <t>Quantidade Vazio</t>
+  </si>
+  <si>
+    <t>Total 82</t>
   </si>
 </sst>
 </file>
@@ -785,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C64"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1506,6 +1510,436 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A83"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>460371</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>393512</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>617112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>557223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>486657</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>664283</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>504864</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>373736</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>655270</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>214162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>491249</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>524992</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>928539</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>930916</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>72862</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>91089</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>113944</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>195564</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>573385</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>624534</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>867398</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>30794</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>625115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>630294</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>630440</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1012388</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>101929</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>669422</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>327571</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>337927</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>698290</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>426532</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>442103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>518204</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>557243</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>726529</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>828295</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>926152</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>931518</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>740091</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>771606</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>406214</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>740978</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>464844</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>541195</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>288917</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>358796</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>780204</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>756742</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>584161</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>836769</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>812304</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>859676</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>836758</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>625736</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>585286</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>862294</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>407542</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>13886</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>177178</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>910504</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>467919</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>186744</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>248022</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>310568</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>419862</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>578470</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>21239312</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>20222726</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>10876194</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>10532189</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>20245604</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>11149425</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>10419702</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>10161268</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>10226764</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>21140976</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>10747120</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>10821051</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>10918535</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>20544139</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>20001614</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D63"/>
   <sheetViews>

</xml_diff>

<commit_message>
Análise inicial de  Dados e Tratamento de Dados
</commit_message>
<xml_diff>
--- a/Tratamento de Dados.xlsx
+++ b/Tratamento de Dados.xlsx
@@ -13,8 +13,10 @@
   </bookViews>
   <sheets>
     <sheet name="Colunas e Relação com Vazio" sheetId="1" r:id="rId1"/>
-    <sheet name="Linhas com Satisfação 99" sheetId="3" r:id="rId2"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId3"/>
+    <sheet name="Correlação" sheetId="5" r:id="rId2"/>
+    <sheet name="Satisfação" sheetId="4" r:id="rId3"/>
+    <sheet name="Linhas com Satisfação 99" sheetId="3" r:id="rId4"/>
+    <sheet name="Plan2" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="140">
   <si>
     <t>IDTNS</t>
   </si>
@@ -437,13 +439,29 @@
   </si>
   <si>
     <t>Total 82</t>
+  </si>
+  <si>
+    <t>Nota</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>NaN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -484,10 +502,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -507,9 +526,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -787,10 +812,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C26" sqref="A26:C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -976,7 +1001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -987,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -998,7 +1023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -1009,7 +1034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
@@ -1020,7 +1045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -1031,7 +1056,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -1042,7 +1067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
@@ -1053,7 +1078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
@@ -1064,7 +1089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
@@ -1075,7 +1100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
@@ -1086,7 +1111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
@@ -1097,7 +1122,7 @@
         <v>33092</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
@@ -1108,7 +1133,7 @@
         <v>92062</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
@@ -1119,7 +1144,7 @@
         <v>127833</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
@@ -1129,8 +1154,12 @@
       <c r="C30" s="3">
         <v>130162</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="1">
+        <f>147777 - C30</f>
+        <v>17615</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>29</v>
       </c>
@@ -1141,7 +1170,7 @@
         <v>33092</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>30</v>
       </c>
@@ -1511,9 +1540,1089 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="9" t="str">
+        <f>VLOOKUP(A1,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Nível de satisfação geral do entrevistado com a prestadora citada </v>
+      </c>
+      <c r="C1" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="9" t="str">
+        <f>VLOOKUP(A2,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Notas atribuídas à cobrança de valores na conta de acordo com o contratado </v>
+      </c>
+      <c r="C2" s="8">
+        <v>0.46367599999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="9" t="str">
+        <f>VLOOKUP(A3,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Notas atribuídas à capacidade de manter a conexão sem quedas. </v>
+      </c>
+      <c r="C3" s="8">
+        <v>0.40635900000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="9" t="str">
+        <f>VLOOKUP(A4,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Ocorre somente em caso de SIM ter sido escolhido em (E7). Nota atribuída à resolução do problema de funcionamento da internet fixa  </v>
+      </c>
+      <c r="C4" s="8">
+        <v>0.36703400000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="9" t="str">
+        <f>VLOOKUP(A5,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Notas atribuídas à velocidade de navegação. </v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.31817000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="9" t="str">
+        <f>VLOOKUP(A6,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Notas atribuídas à qualidade do Atendimento Telefônico da operadora</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.24831800000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="9" t="str">
+        <f>VLOOKUP(A7,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Nota atribuída com respeito ao comprometimento da operadora em cumprir o que foi prometido e divulgado em sua publicidade. </v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.24438199999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="9" t="str">
+        <f>VLOOKUP(A8,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Qualidade do reparo do serviço. </v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.24240200000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="9" t="str">
+        <f>VLOOKUP(A9,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Nota atribuída com respeito à facilidade de entendimento dos planos e serviços contratados </v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.234768</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="9" t="str">
+        <f>VLOOKUP(A10,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Nota Atribuita ao tempo de Espera</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.23469999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="9" t="str">
+        <f>VLOOKUP(A11,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve">  Descreve se o entrevistado entrou em contato com a operadora para falar sobre problemas de funcionamento da internet fixa </v>
+      </c>
+      <c r="C11" s="8">
+        <v>0.21820000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="9" t="str">
+        <f>VLOOKUP(A12,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Notas atribuídas à capacidade de esclarecimento por parte dos atendentes</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.21807399999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="9" t="str">
+        <f>VLOOKUP(A13,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Ocorre somente em caso de SIM ter sido escolhido em (E1). Nota atribuída à resolução do problema de cobrança da prestadora citada. </v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.21734500000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="9" t="str">
+        <f>VLOOKUP(A14,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve">  Ocorre somente em caso de SIM ter sido escolhido em (E3). Nota atribuída à resolução da alteração do plano ou condição comercial. </v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.19830700000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="9" t="str">
+        <f>VLOOKUP(A15,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Cumprimento do prazo acordado para instalação. </v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.19172400000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="9" t="str">
+        <f>VLOOKUP(A16,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Notas atribuídas à necessidade de repetir a demanda</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.18455299999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="9" t="str">
+        <f>VLOOKUP(A17,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Descreve se o usuário solicitou algum tipo de reparo na sua internet fixa nos 6 meses anteriores à pesquisa </v>
+      </c>
+      <c r="C17" s="8">
+        <v>0.17915</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="9" t="str">
+        <f>VLOOKUP(A18,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Qualidade da instalação do serviço. </v>
+      </c>
+      <c r="C18" s="8">
+        <v>0.173761</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="9" t="str">
+        <f>VLOOKUP(A19,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Cumprimento do prazo acordado para reparo. </v>
+      </c>
+      <c r="C19" s="8">
+        <v>0.170991</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="9" t="str">
+        <f>VLOOKUP(A20,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Notas atribuídas à cobrança dos valores na conta de acordo com o contratado </v>
+      </c>
+      <c r="C20" s="8">
+        <v>0.16100400000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="9" t="str">
+        <f>VLOOKUP(A21,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Notas atribuídas ao tempo de espera entre a solicitação de instalação e a visita do técnico.  </v>
+      </c>
+      <c r="C21" s="8">
+        <v>0.15094399999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="9" t="str">
+        <f>VLOOKUP(A22,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Descreve se o entrevistado entrou em contato com a operadora para cancelar serviços ou pacotes  </v>
+      </c>
+      <c r="C22" s="8">
+        <v>0.13791500000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="9" t="str">
+        <f>VLOOKUP(A23,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Descreve se o entrevistado entrou em contato com a operadora para falar sobre algum problema de cobrança nos 6 meses anteriores à pesquisa. </v>
+      </c>
+      <c r="C23" s="8">
+        <v>0.13303300000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="9" t="str">
+        <f>VLOOKUP(A24,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve">  Notas atribuídas à qualidade do Atendimento pela Internet da operadora</v>
+      </c>
+      <c r="C24" s="8">
+        <v>0.130162</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="9" t="str">
+        <f>VLOOKUP(A25,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Ocorre somente em caso de SIM ter sido escolhido em (E5). Nota atribuída à resolução do pedido de cancelamento de serviços ou pacotes </v>
+      </c>
+      <c r="C25" s="8">
+        <v>0.12554699999999999</v>
+      </c>
+      <c r="H25" t="s">
+        <v>47</v>
+      </c>
+      <c r="I25">
+        <v>9.1004000000000002E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="9" t="str">
+        <f>VLOOKUP(A26,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Notas atribuídas à clareza das informações na conta. </v>
+      </c>
+      <c r="C26" s="8">
+        <v>0.109969</v>
+      </c>
+      <c r="H26" t="s">
+        <v>36</v>
+      </c>
+      <c r="I26">
+        <v>6.9405999999999995E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="9" t="str">
+        <f>VLOOKUP(A27,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Notas atribuídas ao tempo de espera entre a solicitação de reparo e a visita do técnico. </v>
+      </c>
+      <c r="C27">
+        <v>9.1004000000000002E-2</v>
+      </c>
+      <c r="H27" t="s">
+        <v>12</v>
+      </c>
+      <c r="I27">
+        <v>3.3274999999999999E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28" s="9" t="str">
+        <f>VLOOKUP(A28,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Descreve se o usuário entrou em contato com a prestadora citada para alterar o plano ou alguma condição comercial nos 6 meses anteriores à pesquisa  </v>
+      </c>
+      <c r="C28">
+        <v>6.9405999999999995E-2</v>
+      </c>
+      <c r="H28" t="s">
+        <v>60</v>
+      </c>
+      <c r="I28">
+        <v>3.2423E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="9" t="str">
+        <f>VLOOKUP(A29,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> O entrevistado é o responsável pelo pagamento dos gastos da internet fixa da prestadora citada </v>
+      </c>
+      <c r="C29">
+        <v>3.3274999999999999E-2</v>
+      </c>
+      <c r="H29" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29">
+        <v>2.9319999999999999E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="9" t="str">
+        <f>VLOOKUP(A30,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve">  : Autorização para identificação das respostas para a empresa que solicitou a pesquisa (2015) ou para a Anatel (a partir de 2016). </v>
+      </c>
+      <c r="C30">
+        <v>3.2423E-2</v>
+      </c>
+      <c r="H30" t="s">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>1.4933E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="9" t="str">
+        <f>VLOOKUP(A31,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Área de Trabalho do Entrevistado </v>
+      </c>
+      <c r="C31">
+        <v>2.9319999999999999E-2</v>
+      </c>
+      <c r="H31" t="s">
+        <v>61</v>
+      </c>
+      <c r="I31">
+        <v>1.4855E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="9" t="str">
+        <f>VLOOKUP(A32,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Identificação  </v>
+      </c>
+      <c r="C32">
+        <v>1.4933E-2</v>
+      </c>
+      <c r="H32" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32">
+        <v>1.1804E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="9" t="str">
+        <f>VLOOKUP(A33,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve">  Autorização para identificação das respostas para a operadora citada.  </v>
+      </c>
+      <c r="C33">
+        <v>1.4855E-2</v>
+      </c>
+      <c r="H33" t="s">
+        <v>50</v>
+      </c>
+      <c r="I33">
+        <v>6.0959999999999999E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="9" t="str">
+        <f>VLOOKUP(A34,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Reposta caso recusa de responder a Q7 </v>
+      </c>
+      <c r="C34">
+        <v>1.1804E-2</v>
+      </c>
+      <c r="H34" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34">
+        <v>4.8040000000000001E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" s="9" t="str">
+        <f>VLOOKUP(A35,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Existência de outra operadora que ofereça o mesmo serviço da atual</v>
+      </c>
+      <c r="C35">
+        <v>6.0959999999999999E-3</v>
+      </c>
+      <c r="H35" t="s">
+        <v>59</v>
+      </c>
+      <c r="I35">
+        <v>2.6710000000000002E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="9" t="str">
+        <f>VLOOKUP(A36,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Idade </v>
+      </c>
+      <c r="C36">
+        <v>4.8040000000000001E-3</v>
+      </c>
+      <c r="H36" t="s">
+        <v>55</v>
+      </c>
+      <c r="I36">
+        <v>-3.9569999999999996E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="9" t="str">
+        <f>VLOOKUP(A37,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Não Identificado no Gloassario </v>
+      </c>
+      <c r="C37">
+        <v>2.6710000000000002E-3</v>
+      </c>
+      <c r="H37" t="s">
+        <v>56</v>
+      </c>
+      <c r="I37">
+        <v>-5.4549999999999998E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="9" t="str">
+        <f>VLOOKUP(A38,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Código IBGE </v>
+      </c>
+      <c r="C38">
+        <v>-3.9569999999999996E-3</v>
+      </c>
+      <c r="H38" t="s">
+        <v>58</v>
+      </c>
+      <c r="I38">
+        <v>-7.3400000000000002E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="9" t="str">
+        <f>VLOOKUP(A39,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Quantidade de pessoas residentes que contribuem com a renda total do domicílio: o entrevistador anota o valor conforme informado pelo entrevistado </v>
+      </c>
+      <c r="C39">
+        <v>-5.4549999999999998E-3</v>
+      </c>
+      <c r="H39" t="s">
+        <v>53</v>
+      </c>
+      <c r="I39">
+        <v>-7.7489999999999998E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" s="9" t="str">
+        <f>VLOOKUP(A40,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Depois de respondida a questão H2 ou em caso de recusa de identificação correta da renda</v>
+      </c>
+      <c r="C40">
+        <v>-7.3400000000000002E-3</v>
+      </c>
+      <c r="H40" t="s">
+        <v>62</v>
+      </c>
+      <c r="I40">
+        <v>-8.1580000000000003E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" s="9" t="str">
+        <f>VLOOKUP(A41,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Contrato inclui Telefonia Fixa</v>
+      </c>
+      <c r="C41">
+        <v>-7.7489999999999998E-3</v>
+      </c>
+      <c r="H41" t="s">
+        <v>57</v>
+      </c>
+      <c r="I41">
+        <v>-1.3141E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="9" t="str">
+        <f>VLOOKUP(A42,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Peso do estrato (UF x prestadora) na amostra</v>
+      </c>
+      <c r="C42">
+        <v>-8.1580000000000003E-3</v>
+      </c>
+      <c r="H42" t="s">
+        <v>42</v>
+      </c>
+      <c r="I42">
+        <v>-1.5216E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" s="9" t="str">
+        <f>VLOOKUP(A43,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Renda mensal familiar: o entrevistador anota o valor conforme informado pelo entrevistado </v>
+      </c>
+      <c r="C43">
+        <v>-1.3141E-2</v>
+      </c>
+      <c r="H43" t="s">
+        <v>52</v>
+      </c>
+      <c r="I43">
+        <v>-1.738E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="9" t="str">
+        <f>VLOOKUP(A44,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve">  Descreve se o usuário solicitou instalação de internet fixa em seu endereço atual nos 6 meses anteriores à pesquisa.  </v>
+      </c>
+      <c r="C44">
+        <v>-1.5216E-2</v>
+      </c>
+      <c r="H44" t="s">
+        <v>51</v>
+      </c>
+      <c r="I44">
+        <v>-1.9531E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="9" t="str">
+        <f>VLOOKUP(A45,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve">  Contrato inclui Telefonia Móvel</v>
+      </c>
+      <c r="C45">
+        <v>-1.738E-2</v>
+      </c>
+      <c r="H45" t="s">
+        <v>5</v>
+      </c>
+      <c r="I45">
+        <v>-2.2051000000000001E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46" s="9" t="str">
+        <f>VLOOKUP(A46,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve">  Contrato inclui TV por assinatura</v>
+      </c>
+      <c r="C46">
+        <v>-1.9531E-2</v>
+      </c>
+      <c r="H46" t="s">
+        <v>16</v>
+      </c>
+      <c r="I46">
+        <v>-3.3201000000000001E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="9" t="str">
+        <f>VLOOKUP(A47,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Ano </v>
+      </c>
+      <c r="C47">
+        <v>-2.2051000000000001E-2</v>
+      </c>
+      <c r="H47" t="s">
+        <v>6</v>
+      </c>
+      <c r="I47" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48" s="9" t="str">
+        <f>VLOOKUP(A48,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Sexo </v>
+      </c>
+      <c r="C48">
+        <v>-3.3201000000000001E-2</v>
+      </c>
+      <c r="H48" t="s">
+        <v>8</v>
+      </c>
+      <c r="I48" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" s="9" t="str">
+        <f>VLOOKUP(A49,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Interesse em participar da Pesquisa </v>
+      </c>
+      <c r="C49" t="s">
+        <v>139</v>
+      </c>
+      <c r="H49" t="s">
+        <v>9</v>
+      </c>
+      <c r="I49" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="9" t="str">
+        <f>VLOOKUP(A50,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Área de Trabalho do Entrevistado Atualizado Pós 2016 </v>
+      </c>
+      <c r="C50" t="s">
+        <v>139</v>
+      </c>
+      <c r="H50" t="s">
+        <v>10</v>
+      </c>
+      <c r="I50" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" s="9" t="str">
+        <f>VLOOKUP(A51,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Área de Trabalho do Entrevistado Atualizado Pós 2016 </v>
+      </c>
+      <c r="C51" t="s">
+        <v>139</v>
+      </c>
+      <c r="H51" t="s">
+        <v>11</v>
+      </c>
+      <c r="I51" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="9" t="str">
+        <f>VLOOKUP(A52,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Usuário é cliente de internet fixa </v>
+      </c>
+      <c r="C52" t="s">
+        <v>139</v>
+      </c>
+      <c r="H52" t="s">
+        <v>13</v>
+      </c>
+      <c r="I52" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>11</v>
+      </c>
+      <c r="B53" s="9" t="str">
+        <f>VLOOKUP(A53,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve">  O entrevistado é um dos principais usuários da internet fixa da prestadora citada dentro da residência?  </v>
+      </c>
+      <c r="C53" t="s">
+        <v>139</v>
+      </c>
+      <c r="H53" t="s">
+        <v>25</v>
+      </c>
+      <c r="I53" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" s="9" t="str">
+        <f>VLOOKUP(A54,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> Pessoa Física ou Pessoa Jurídica </v>
+      </c>
+      <c r="C54" t="s">
+        <v>139</v>
+      </c>
+      <c r="H54" t="s">
+        <v>26</v>
+      </c>
+      <c r="I54" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" s="9" t="str">
+        <f>VLOOKUP(A55,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> o entrevistado utilizou o Atendimento Telefônico da prestadora nos seis meses anteriores à pesquisa? </v>
+      </c>
+      <c r="C55" t="s">
+        <v>139</v>
+      </c>
+      <c r="H55" t="s">
+        <v>27</v>
+      </c>
+      <c r="I55" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" s="9" t="str">
+        <f>VLOOKUP(A56,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve">  o entrevistado utilizou o Atendimento pela Internet da prestadora nos seis meses anteriores à pesquisa? </v>
+      </c>
+      <c r="C56" t="s">
+        <v>139</v>
+      </c>
+      <c r="H56" t="s">
+        <v>28</v>
+      </c>
+      <c r="I56" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" s="9" t="str">
+        <f>VLOOKUP(A57,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve">  o entrevistado utilizou o Atendimento na Loja da prestadora nos seis meses anteriores à pesquisa? </v>
+      </c>
+      <c r="C57" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>28</v>
+      </c>
+      <c r="B58" s="9" t="str">
+        <f>VLOOKUP(A58,'Colunas e Relação com Vazio'!A:C,2,FALSE)</f>
+        <v xml:space="preserve"> o entrevistado não utilizou os canais da prestadora citados anteriormente nos seis meses anteriores à pesquisa? </v>
+      </c>
+      <c r="C58" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>31403</v>
+      </c>
+      <c r="C2" s="7">
+        <f>B2/$D$2</f>
+        <v>0.21250262219425214</v>
+      </c>
+      <c r="D2">
+        <v>147777</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>26085</v>
+      </c>
+      <c r="C3" s="7">
+        <f t="shared" ref="C3:C13" si="0">B3/$D$2</f>
+        <v>0.17651596662538827</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>21823</v>
+      </c>
+      <c r="C4" s="7">
+        <f t="shared" si="0"/>
+        <v>0.14767521332819045</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>16662</v>
+      </c>
+      <c r="C5" s="7">
+        <f t="shared" si="0"/>
+        <v>0.11275096936600418</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>14279</v>
+      </c>
+      <c r="C6" s="7">
+        <f t="shared" si="0"/>
+        <v>9.6625320584394048E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>12078</v>
+      </c>
+      <c r="C7" s="7">
+        <f t="shared" si="0"/>
+        <v>8.1731257232180915E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>7464</v>
+      </c>
+      <c r="C8" s="7">
+        <f t="shared" si="0"/>
+        <v>5.0508536511094416E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>7260</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" si="0"/>
+        <v>4.912807811770438E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>5136</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" si="0"/>
+        <v>3.4755070139466902E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>3629</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="0"/>
+        <v>2.4557272105943415E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>1876</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2694803656861351E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>99</v>
+      </c>
+      <c r="B13">
+        <v>82</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="0"/>
+        <v>5.5489013851952609E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1939,7 +3048,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D63"/>
   <sheetViews>

</xml_diff>

<commit_message>
HeatMap para análise inicial de dados
</commit_message>
<xml_diff>
--- a/Tratamento de Dados.xlsx
+++ b/Tratamento de Dados.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Colunas e Relação com Vazio" sheetId="1" r:id="rId1"/>
-    <sheet name="Correlação" sheetId="5" r:id="rId2"/>
-    <sheet name="Satisfação" sheetId="4" r:id="rId3"/>
-    <sheet name="Linhas com Satisfação 99" sheetId="3" r:id="rId4"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId5"/>
+    <sheet name="Plan1" sheetId="6" r:id="rId2"/>
+    <sheet name="Correlação" sheetId="5" r:id="rId3"/>
+    <sheet name="Satisfação" sheetId="4" r:id="rId4"/>
+    <sheet name="Linhas com Satisfação 99" sheetId="3" r:id="rId5"/>
+    <sheet name="Plan2" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="140">
   <si>
     <t>IDTNS</t>
   </si>
@@ -814,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C26" sqref="A26:C26"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1540,10 +1541,230 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>3</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <f>2^B1</f>
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:E2" si="0">2^C1</f>
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f>B4*$B$2+C4*$C$2+D4*$D$2+E4*$E$2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:F17" si="1">B5*$B$2+C5*$C$2+D5*$D$2+E5*$E$2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <f>B11*$B$2+C11*$C$2+D11*$D$2+E11*$E$2</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1894,7 +2115,7 @@
         <v>3.3274999999999999E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1912,7 +2133,7 @@
         <v>3.2423E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -1930,7 +2151,7 @@
         <v>2.9319999999999999E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -1948,7 +2169,7 @@
         <v>1.4933E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1966,7 +2187,7 @@
         <v>1.4855E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -2002,7 +2223,7 @@
         <v>6.0959999999999999E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -2038,7 +2259,7 @@
         <v>2.6710000000000002E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -2056,7 +2277,7 @@
         <v>-3.9569999999999996E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>59</v>
       </c>
@@ -2074,7 +2295,7 @@
         <v>-5.4549999999999998E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -2092,7 +2313,7 @@
         <v>-7.3400000000000002E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>56</v>
       </c>
@@ -2110,7 +2331,7 @@
         <v>-7.7489999999999998E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>58</v>
       </c>
@@ -2128,7 +2349,7 @@
         <v>-8.1580000000000003E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -2146,7 +2367,7 @@
         <v>-1.3141E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>62</v>
       </c>
@@ -2182,7 +2403,7 @@
         <v>-1.738E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2200,7 +2421,7 @@
         <v>-1.9531E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>52</v>
       </c>
@@ -2218,7 +2439,7 @@
         <v>-2.2051000000000001E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>51</v>
       </c>
@@ -2236,7 +2457,7 @@
         <v>-3.3201000000000001E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -2254,7 +2475,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -2272,7 +2493,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -2326,7 +2547,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -2344,7 +2565,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -2362,7 +2583,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>13</v>
       </c>
@@ -2380,7 +2601,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>25</v>
       </c>
@@ -2398,7 +2619,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>26</v>
       </c>
@@ -2416,7 +2637,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>27</v>
       </c>
@@ -2428,7 +2649,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>28</v>
       </c>
@@ -2445,7 +2666,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -2618,7 +2839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A83"/>
   <sheetViews>
@@ -3048,12 +3269,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B63"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Graficos de Satisfação Média
</commit_message>
<xml_diff>
--- a/Tratamento de Dados.xlsx
+++ b/Tratamento de Dados.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Colunas e Relação com Vazio" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,11 @@
     <sheet name="Satisfação" sheetId="4" r:id="rId4"/>
     <sheet name="Linhas com Satisfação 99" sheetId="3" r:id="rId5"/>
     <sheet name="Plan2" sheetId="2" r:id="rId6"/>
+    <sheet name="Plan3" sheetId="7" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Plan3!$A$1:$I$64</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="262">
   <si>
     <t>IDTNS</t>
   </si>
@@ -449,6 +453,372 @@
   </si>
   <si>
     <t>NaN</t>
+  </si>
+  <si>
+    <t>Participação da Pesquisa</t>
+  </si>
+  <si>
+    <t>Área de Trabalho</t>
+  </si>
+  <si>
+    <t>Área de Trabalho pós 2016 1</t>
+  </si>
+  <si>
+    <t>Área de Trabalho pós 2016 2</t>
+  </si>
+  <si>
+    <t>Cliente de Internet fixa</t>
+  </si>
+  <si>
+    <t>Principal Usuário</t>
+  </si>
+  <si>
+    <t>Responsável pelo Pagamento</t>
+  </si>
+  <si>
+    <t>Pessoa Física ou Jurídica</t>
+  </si>
+  <si>
+    <t>Idade</t>
+  </si>
+  <si>
+    <t>Recusa Idade</t>
+  </si>
+  <si>
+    <t>Sexo</t>
+  </si>
+  <si>
+    <t>SAT Geral</t>
+  </si>
+  <si>
+    <t>SAT Entendimento dos Planos</t>
+  </si>
+  <si>
+    <t>SAT Comprometimento com o prometido</t>
+  </si>
+  <si>
+    <t>SAT Conexões sem Queda</t>
+  </si>
+  <si>
+    <t>SAT velocidade</t>
+  </si>
+  <si>
+    <t>SAT Cobrança Funcionamento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAT Cobrança Contas a Pagar </t>
+  </si>
+  <si>
+    <t>SAT Clareza Info da Conta</t>
+  </si>
+  <si>
+    <t>Usou atendimento Internet ?</t>
+  </si>
+  <si>
+    <t>Usou atendimento telefonico ?</t>
+  </si>
+  <si>
+    <t>Usou atendimento local Físico ?</t>
+  </si>
+  <si>
+    <t>Usou atendimento ?</t>
+  </si>
+  <si>
+    <t>SAT tempo de espera Atendimento</t>
+  </si>
+  <si>
+    <t>SAT Necessidade Repetição</t>
+  </si>
+  <si>
+    <t>SAT Esclarecimentos Atendentes</t>
+  </si>
+  <si>
+    <t>SAT Atendimento Telefônico</t>
+  </si>
+  <si>
+    <t>SAT Atendimento Internet</t>
+  </si>
+  <si>
+    <t>Entrou em contato devido a problema de cobrança</t>
+  </si>
+  <si>
+    <t>SAT Resolução Problema Cobrança</t>
+  </si>
+  <si>
+    <t>Entrou em Contato para Alterar Plano</t>
+  </si>
+  <si>
+    <t>SAT Resolução Alteração</t>
+  </si>
+  <si>
+    <t>Entrou em Contato para Cancelar</t>
+  </si>
+  <si>
+    <t>SAT Resolução Cancelamento</t>
+  </si>
+  <si>
+    <t>Entrou em Contato para Problemas</t>
+  </si>
+  <si>
+    <t>SAT a resolução do Problema</t>
+  </si>
+  <si>
+    <t>Solicitou instalação de internet fixa</t>
+  </si>
+  <si>
+    <t>SAT Solicitação de Instalação</t>
+  </si>
+  <si>
+    <t>SAT Prazo Instalação</t>
+  </si>
+  <si>
+    <t>SAT Qualidade Instalação</t>
+  </si>
+  <si>
+    <t>Solicito reparos</t>
+  </si>
+  <si>
+    <t>SAT Reparos</t>
+  </si>
+  <si>
+    <t>SAT Prazo Reparos</t>
+  </si>
+  <si>
+    <t>SAT Qualidade Reparos</t>
+  </si>
+  <si>
+    <t>Existência de Outra Operadora</t>
+  </si>
+  <si>
+    <t>Inclui TV?</t>
+  </si>
+  <si>
+    <t>Inclui Telefonia Móvel?</t>
+  </si>
+  <si>
+    <t>Inclui Telefone Fixo</t>
+  </si>
+  <si>
+    <t>Município</t>
+  </si>
+  <si>
+    <t>IBGE</t>
+  </si>
+  <si>
+    <t>Quantidade de pessoas</t>
+  </si>
+  <si>
+    <t>Renda</t>
+  </si>
+  <si>
+    <t>Recusa Renda</t>
+  </si>
+  <si>
+    <t>Autorização 2</t>
+  </si>
+  <si>
+    <t>Autorização 1</t>
+  </si>
+  <si>
+    <t>Glossario["IDTNS"] </t>
+  </si>
+  <si>
+    <t>Glossario["TIPO"] </t>
+  </si>
+  <si>
+    <t>Glossario["OPERADORA"] </t>
+  </si>
+  <si>
+    <t>Glossario["ESTADO"] </t>
+  </si>
+  <si>
+    <t>Glossario["DATA"] </t>
+  </si>
+  <si>
+    <t>Glossario["ANO_BASE"] </t>
+  </si>
+  <si>
+    <t>Glossario["Q1"] </t>
+  </si>
+  <si>
+    <t>Glossario["Q2"] </t>
+  </si>
+  <si>
+    <t>Glossario["Q2_1"] </t>
+  </si>
+  <si>
+    <t>Glossario["Q2_2"] </t>
+  </si>
+  <si>
+    <t>Glossario["Q3"] </t>
+  </si>
+  <si>
+    <t>Glossario["Q4"] </t>
+  </si>
+  <si>
+    <t>Glossario["Q5"] </t>
+  </si>
+  <si>
+    <t>Glossario["Q6"] </t>
+  </si>
+  <si>
+    <t>Glossario["Q7"] </t>
+  </si>
+  <si>
+    <t>Glossario["Q7a"] </t>
+  </si>
+  <si>
+    <t>Glossario["Q8"] </t>
+  </si>
+  <si>
+    <t>Glossario["J1"] </t>
+  </si>
+  <si>
+    <t>Glossario["B1_1"] </t>
+  </si>
+  <si>
+    <t>Glossario["B1_2"] </t>
+  </si>
+  <si>
+    <t>Glossario["C1_1"] </t>
+  </si>
+  <si>
+    <t>Glossario["C1_2"] </t>
+  </si>
+  <si>
+    <t>Glossario["C1_3"] </t>
+  </si>
+  <si>
+    <t>Glossario["D1_1"] </t>
+  </si>
+  <si>
+    <t>Glossario["D1_2"] </t>
+  </si>
+  <si>
+    <t>Glossario["A1_1"] </t>
+  </si>
+  <si>
+    <t>Glossario["A1_2"] </t>
+  </si>
+  <si>
+    <t>Glossario["A1_3"] </t>
+  </si>
+  <si>
+    <t>Glossario["A1_4"] </t>
+  </si>
+  <si>
+    <t>Glossario["A2_1"] </t>
+  </si>
+  <si>
+    <t>Glossario["A2_2"] </t>
+  </si>
+  <si>
+    <t>Glossario["A2_3"] </t>
+  </si>
+  <si>
+    <t>Glossario["A3"] </t>
+  </si>
+  <si>
+    <t>Glossario["A4"] </t>
+  </si>
+  <si>
+    <t>Glossario["E1"] </t>
+  </si>
+  <si>
+    <t>Glossario["E2"] </t>
+  </si>
+  <si>
+    <t>Glossario["E3"] </t>
+  </si>
+  <si>
+    <t>Glossario["E4"] </t>
+  </si>
+  <si>
+    <t>Glossario["E5"] </t>
+  </si>
+  <si>
+    <t>Glossario["E6"] </t>
+  </si>
+  <si>
+    <t>Glossario["E7"] </t>
+  </si>
+  <si>
+    <t>Glossario["E8"] </t>
+  </si>
+  <si>
+    <t>Glossario["F1"] </t>
+  </si>
+  <si>
+    <t>Glossario["F2_1"] </t>
+  </si>
+  <si>
+    <t>Glossario["F2_2"] </t>
+  </si>
+  <si>
+    <t>Glossario["F2_3"] </t>
+  </si>
+  <si>
+    <t>Glossario["F3"] </t>
+  </si>
+  <si>
+    <t>Glossario["F4_1"] </t>
+  </si>
+  <si>
+    <t>Glossario["F4_2"] </t>
+  </si>
+  <si>
+    <t>Glossario["F4_3"] </t>
+  </si>
+  <si>
+    <t>Glossario["G1"] </t>
+  </si>
+  <si>
+    <t>Glossario["G2_1"] </t>
+  </si>
+  <si>
+    <t>Glossario["G2_2"] </t>
+  </si>
+  <si>
+    <t>Glossario["G2_3"] </t>
+  </si>
+  <si>
+    <t>Glossario["H0"] </t>
+  </si>
+  <si>
+    <t>Glossario["H1"] </t>
+  </si>
+  <si>
+    <t>Glossario["H2"] </t>
+  </si>
+  <si>
+    <t>Glossario["H2a"] </t>
+  </si>
+  <si>
+    <t>Glossario["H3"] </t>
+  </si>
+  <si>
+    <t>Glossario["I1"] </t>
+  </si>
+  <si>
+    <t>Glossario["I2"] </t>
+  </si>
+  <si>
+    <t>Glossario["PESO"] </t>
+  </si>
+  <si>
+    <t>Glossario["COD_IBGE"] </t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>Data_Reshaped.drop(</t>
+  </si>
+  <si>
+    <t>, inplace= True, axis = 1)</t>
   </si>
 </sst>
 </file>
@@ -1543,7 +1913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3:F11"/>
     </sheetView>
   </sheetViews>
@@ -3271,556 +3641,2607 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:B29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B63" sqref="B1:B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="139.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="139.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>141</v>
+      </c>
+      <c r="C8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>143</v>
+      </c>
+      <c r="C10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C15" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>151</v>
+      </c>
+      <c r="C18" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>152</v>
+      </c>
+      <c r="C19" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>153</v>
+      </c>
+      <c r="C20" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C22" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>157</v>
+      </c>
+      <c r="C24" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>158</v>
+      </c>
+      <c r="C25" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>160</v>
+      </c>
+      <c r="C26" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>159</v>
+      </c>
+      <c r="C27" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>161</v>
+      </c>
+      <c r="C28" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>162</v>
+      </c>
+      <c r="C29" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>163</v>
+      </c>
+      <c r="C30" t="s">
         <v>99</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" t="s">
         <v>100</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>165</v>
+      </c>
+      <c r="C32" t="s">
         <v>101</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>64</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>166</v>
+      </c>
+      <c r="C33" t="s">
         <v>102</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>167</v>
+      </c>
+      <c r="C34" t="s">
         <v>103</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
       <c r="B35" t="s">
+        <v>168</v>
+      </c>
+      <c r="C35" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>169</v>
+      </c>
+      <c r="C36" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>170</v>
+      </c>
+      <c r="C37" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>171</v>
+      </c>
+      <c r="C38" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>172</v>
+      </c>
+      <c r="C39" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
       <c r="B40" t="s">
+        <v>173</v>
+      </c>
+      <c r="C40" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>174</v>
+      </c>
+      <c r="C41" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>175</v>
+      </c>
+      <c r="C42" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>176</v>
+      </c>
+      <c r="C43" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>177</v>
+      </c>
+      <c r="C44" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>178</v>
+      </c>
+      <c r="C45" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>179</v>
+      </c>
+      <c r="C46" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>180</v>
+      </c>
+      <c r="C47" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
       <c r="B48" t="s">
+        <v>181</v>
+      </c>
+      <c r="C48" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
       <c r="B49" t="s">
+        <v>182</v>
+      </c>
+      <c r="C49" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
       <c r="B50" t="s">
+        <v>183</v>
+      </c>
+      <c r="C50" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
       <c r="B51" t="s">
+        <v>184</v>
+      </c>
+      <c r="C51" t="s">
         <v>120</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
       <c r="B52" t="s">
+        <v>185</v>
+      </c>
+      <c r="C52" t="s">
         <v>121</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>186</v>
+      </c>
+      <c r="C53" t="s">
         <v>122</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
       <c r="B54" t="s">
+        <v>187</v>
+      </c>
+      <c r="C54" t="s">
         <v>123</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
       <c r="B55" t="s">
+        <v>188</v>
+      </c>
+      <c r="C55" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
       <c r="B56" t="s">
+        <v>189</v>
+      </c>
+      <c r="C56" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
       <c r="B57" t="s">
+        <v>190</v>
+      </c>
+      <c r="C57" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
       <c r="B58" t="s">
+        <v>191</v>
+      </c>
+      <c r="C58" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
       <c r="B59" t="s">
+        <v>192</v>
+      </c>
+      <c r="C59" t="s">
         <v>128</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
       <c r="B60" t="s">
+        <v>59</v>
+      </c>
+      <c r="C60" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
       <c r="B61" t="s">
+        <v>194</v>
+      </c>
+      <c r="C61" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>61</v>
       </c>
       <c r="B62" t="s">
+        <v>193</v>
+      </c>
+      <c r="C62" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>62</v>
       </c>
       <c r="B63" t="s">
+        <v>62</v>
+      </c>
+      <c r="C63" t="s">
         <v>132</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.28515625" customWidth="1"/>
+    <col min="9" max="9" width="46.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>259</v>
+      </c>
+      <c r="D1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C2" t="str">
+        <f>CONCATENATE($C$1,I2,$D$1)</f>
+        <v>" Identificação  "</v>
+      </c>
+      <c r="D2" t="str">
+        <f>CONCATENATE(A2,B2,C2)</f>
+        <v>Glossario["IDTNS"] =" Identificação  "</v>
+      </c>
+      <c r="E2" t="s">
+        <v>260</v>
+      </c>
+      <c r="F2" t="str">
+        <f>CONCATENATE(E2,C2,G2)</f>
+        <v>Data_Reshaped.drop(" Identificação  ", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G2" t="s">
+        <v>261</v>
+      </c>
+      <c r="I2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3" t="s">
+        <v>258</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C64" si="0">CONCATENATE($C$1,I3,$D$1)</f>
+        <v>" Tipo de Serviço  "</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D64" si="1">CONCATENATE(A3,B3,C3)</f>
+        <v>Glossario["TIPO"] =" Tipo de Serviço  "</v>
+      </c>
+      <c r="E3" t="s">
+        <v>260</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F64" si="2">CONCATENATE(E3,C3,G3)</f>
+        <v>Data_Reshaped.drop(" Tipo de Serviço  ", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G3" t="s">
+        <v>261</v>
+      </c>
+      <c r="I3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>" Operadora  "</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["OPERADORA"] =" Operadora  "</v>
+      </c>
+      <c r="E4" t="s">
+        <v>260</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop(" Operadora  ", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G4" t="s">
+        <v>261</v>
+      </c>
+      <c r="I4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>" Estado "</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["ESTADO"] =" Estado "</v>
+      </c>
+      <c r="E5" t="s">
+        <v>260</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop(" Estado ", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G5" t="s">
+        <v>261</v>
+      </c>
+      <c r="I5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>199</v>
+      </c>
+      <c r="B6" t="s">
+        <v>258</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>" Data "</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["DATA"] =" Data "</v>
+      </c>
+      <c r="E6" t="s">
+        <v>260</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop(" Data ", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G6" t="s">
+        <v>261</v>
+      </c>
+      <c r="I6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B7" t="s">
+        <v>258</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>" Ano "</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["ANO_BASE"] =" Ano "</v>
+      </c>
+      <c r="E7" t="s">
+        <v>260</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop(" Ano ", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G7" t="s">
+        <v>261</v>
+      </c>
+      <c r="I7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>"Participação da Pesquisa"</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["Q1"] ="Participação da Pesquisa"</v>
+      </c>
+      <c r="E8" t="s">
+        <v>260</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Participação da Pesquisa", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G8" t="s">
+        <v>261</v>
+      </c>
+      <c r="I8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>202</v>
+      </c>
+      <c r="B9" t="s">
+        <v>258</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>"Área de Trabalho"</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["Q2"] ="Área de Trabalho"</v>
+      </c>
+      <c r="E9" t="s">
+        <v>260</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Área de Trabalho", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G9" t="s">
+        <v>261</v>
+      </c>
+      <c r="I9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>203</v>
+      </c>
+      <c r="B10" t="s">
+        <v>258</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>"Área de Trabalho pós 2016 1"</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["Q2_1"] ="Área de Trabalho pós 2016 1"</v>
+      </c>
+      <c r="E10" t="s">
+        <v>260</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Área de Trabalho pós 2016 1", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G10" t="s">
+        <v>261</v>
+      </c>
+      <c r="I10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B11" t="s">
+        <v>258</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>"Área de Trabalho pós 2016 2"</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["Q2_2"] ="Área de Trabalho pós 2016 2"</v>
+      </c>
+      <c r="E11" t="s">
+        <v>260</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Área de Trabalho pós 2016 2", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G11" t="s">
+        <v>261</v>
+      </c>
+      <c r="I11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>205</v>
+      </c>
+      <c r="B12" t="s">
+        <v>258</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>"Cliente de Internet fixa"</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["Q3"] ="Cliente de Internet fixa"</v>
+      </c>
+      <c r="E12" t="s">
+        <v>260</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Cliente de Internet fixa", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G12" t="s">
+        <v>261</v>
+      </c>
+      <c r="I12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>206</v>
+      </c>
+      <c r="B13" t="s">
+        <v>258</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>"Principal Usuário"</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["Q4"] ="Principal Usuário"</v>
+      </c>
+      <c r="E13" t="s">
+        <v>260</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Principal Usuário", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G13" t="s">
+        <v>261</v>
+      </c>
+      <c r="I13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B14" t="s">
+        <v>258</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>"Responsável pelo Pagamento"</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["Q5"] ="Responsável pelo Pagamento"</v>
+      </c>
+      <c r="E14" t="s">
+        <v>260</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Responsável pelo Pagamento", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G14" t="s">
+        <v>261</v>
+      </c>
+      <c r="I14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>208</v>
+      </c>
+      <c r="B15" t="s">
+        <v>258</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>"Pessoa Física ou Jurídica"</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["Q6"] ="Pessoa Física ou Jurídica"</v>
+      </c>
+      <c r="E15" t="s">
+        <v>260</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Pessoa Física ou Jurídica", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G15" t="s">
+        <v>261</v>
+      </c>
+      <c r="I15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>209</v>
+      </c>
+      <c r="B16" t="s">
+        <v>258</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>"Idade"</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["Q7"] ="Idade"</v>
+      </c>
+      <c r="E16" t="s">
+        <v>260</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Idade", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G16" t="s">
+        <v>261</v>
+      </c>
+      <c r="I16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>210</v>
+      </c>
+      <c r="B17" t="s">
+        <v>258</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>"Recusa Idade"</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["Q7a"] ="Recusa Idade"</v>
+      </c>
+      <c r="E17" t="s">
+        <v>260</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Recusa Idade", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G17" t="s">
+        <v>261</v>
+      </c>
+      <c r="I17" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>211</v>
+      </c>
+      <c r="B18" t="s">
+        <v>258</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>"Sexo"</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["Q8"] ="Sexo"</v>
+      </c>
+      <c r="E18" t="s">
+        <v>260</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Sexo", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G18" t="s">
+        <v>261</v>
+      </c>
+      <c r="I18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>212</v>
+      </c>
+      <c r="B19" t="s">
+        <v>258</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT Geral"</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["J1"] ="SAT Geral"</v>
+      </c>
+      <c r="E19" t="s">
+        <v>260</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT Geral", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G19" t="s">
+        <v>261</v>
+      </c>
+      <c r="I19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>213</v>
+      </c>
+      <c r="B20" t="s">
+        <v>258</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT Entendimento dos Planos"</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["B1_1"] ="SAT Entendimento dos Planos"</v>
+      </c>
+      <c r="E20" t="s">
+        <v>260</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT Entendimento dos Planos", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G20" t="s">
+        <v>261</v>
+      </c>
+      <c r="I20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>214</v>
+      </c>
+      <c r="B21" t="s">
+        <v>258</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT Comprometimento com o prometido"</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["B1_2"] ="SAT Comprometimento com o prometido"</v>
+      </c>
+      <c r="E21" t="s">
+        <v>260</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT Comprometimento com o prometido", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G21" t="s">
+        <v>261</v>
+      </c>
+      <c r="I21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>215</v>
+      </c>
+      <c r="B22" t="s">
+        <v>258</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT Cobrança Funcionamento"</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["C1_1"] ="SAT Cobrança Funcionamento"</v>
+      </c>
+      <c r="E22" t="s">
+        <v>260</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT Cobrança Funcionamento", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G22" t="s">
+        <v>261</v>
+      </c>
+      <c r="I22" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>216</v>
+      </c>
+      <c r="B23" t="s">
+        <v>258</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT Conexões sem Queda"</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["C1_2"] ="SAT Conexões sem Queda"</v>
+      </c>
+      <c r="E23" t="s">
+        <v>260</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT Conexões sem Queda", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G23" t="s">
+        <v>261</v>
+      </c>
+      <c r="I23" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>217</v>
+      </c>
+      <c r="B24" t="s">
+        <v>258</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT velocidade"</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["C1_3"] ="SAT velocidade"</v>
+      </c>
+      <c r="E24" t="s">
+        <v>260</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT velocidade", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G24" t="s">
+        <v>261</v>
+      </c>
+      <c r="I24" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>218</v>
+      </c>
+      <c r="B25" t="s">
+        <v>258</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT Cobrança Contas a Pagar "</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["D1_1"] ="SAT Cobrança Contas a Pagar "</v>
+      </c>
+      <c r="E25" t="s">
+        <v>260</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT Cobrança Contas a Pagar ", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G25" t="s">
+        <v>261</v>
+      </c>
+      <c r="I25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>219</v>
+      </c>
+      <c r="B26" t="s">
+        <v>258</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT Clareza Info da Conta"</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["D1_2"] ="SAT Clareza Info da Conta"</v>
+      </c>
+      <c r="E26" t="s">
+        <v>260</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT Clareza Info da Conta", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G26" t="s">
+        <v>261</v>
+      </c>
+      <c r="I26" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>220</v>
+      </c>
+      <c r="B27" t="s">
+        <v>258</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>"Usou atendimento telefonico ?"</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["A1_1"] ="Usou atendimento telefonico ?"</v>
+      </c>
+      <c r="E27" t="s">
+        <v>260</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Usou atendimento telefonico ?", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G27" t="s">
+        <v>261</v>
+      </c>
+      <c r="I27" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>221</v>
+      </c>
+      <c r="B28" t="s">
+        <v>258</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>"Usou atendimento Internet ?"</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["A1_2"] ="Usou atendimento Internet ?"</v>
+      </c>
+      <c r="E28" t="s">
+        <v>260</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Usou atendimento Internet ?", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G28" t="s">
+        <v>261</v>
+      </c>
+      <c r="I28" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>222</v>
+      </c>
+      <c r="B29" t="s">
+        <v>258</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>"Usou atendimento local Físico ?"</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["A1_3"] ="Usou atendimento local Físico ?"</v>
+      </c>
+      <c r="E29" t="s">
+        <v>260</v>
+      </c>
+      <c r="F29" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Usou atendimento local Físico ?", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G29" t="s">
+        <v>261</v>
+      </c>
+      <c r="I29" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>223</v>
+      </c>
+      <c r="B30" t="s">
+        <v>258</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>"Usou atendimento ?"</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["A1_4"] ="Usou atendimento ?"</v>
+      </c>
+      <c r="E30" t="s">
+        <v>260</v>
+      </c>
+      <c r="F30" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Usou atendimento ?", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G30" t="s">
+        <v>261</v>
+      </c>
+      <c r="I30" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>224</v>
+      </c>
+      <c r="B31" t="s">
+        <v>258</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT tempo de espera Atendimento"</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["A2_1"] ="SAT tempo de espera Atendimento"</v>
+      </c>
+      <c r="E31" t="s">
+        <v>260</v>
+      </c>
+      <c r="F31" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT tempo de espera Atendimento", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G31" t="s">
+        <v>261</v>
+      </c>
+      <c r="I31" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>225</v>
+      </c>
+      <c r="B32" t="s">
+        <v>258</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT Necessidade Repetição"</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["A2_2"] ="SAT Necessidade Repetição"</v>
+      </c>
+      <c r="E32" t="s">
+        <v>260</v>
+      </c>
+      <c r="F32" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT Necessidade Repetição", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G32" t="s">
+        <v>261</v>
+      </c>
+      <c r="I32" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>226</v>
+      </c>
+      <c r="B33" t="s">
+        <v>258</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT Esclarecimentos Atendentes"</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["A2_3"] ="SAT Esclarecimentos Atendentes"</v>
+      </c>
+      <c r="E33" t="s">
+        <v>260</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT Esclarecimentos Atendentes", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G33" t="s">
+        <v>261</v>
+      </c>
+      <c r="I33" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>227</v>
+      </c>
+      <c r="B34" t="s">
+        <v>258</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT Atendimento Telefônico"</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["A3"] ="SAT Atendimento Telefônico"</v>
+      </c>
+      <c r="E34" t="s">
+        <v>260</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT Atendimento Telefônico", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G34" t="s">
+        <v>261</v>
+      </c>
+      <c r="I34" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>228</v>
+      </c>
+      <c r="B35" t="s">
+        <v>258</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT Atendimento Internet"</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["A4"] ="SAT Atendimento Internet"</v>
+      </c>
+      <c r="E35" t="s">
+        <v>260</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT Atendimento Internet", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G35" t="s">
+        <v>261</v>
+      </c>
+      <c r="I35" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>229</v>
+      </c>
+      <c r="B36" t="s">
+        <v>258</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>"Entrou em contato devido a problema de cobrança"</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["E1"] ="Entrou em contato devido a problema de cobrança"</v>
+      </c>
+      <c r="E36" t="s">
+        <v>260</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Entrou em contato devido a problema de cobrança", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G36" t="s">
+        <v>261</v>
+      </c>
+      <c r="I36" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>230</v>
+      </c>
+      <c r="B37" t="s">
+        <v>258</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT Resolução Problema Cobrança"</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["E2"] ="SAT Resolução Problema Cobrança"</v>
+      </c>
+      <c r="E37" t="s">
+        <v>260</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT Resolução Problema Cobrança", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G37" t="s">
+        <v>261</v>
+      </c>
+      <c r="I37" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>231</v>
+      </c>
+      <c r="B38" t="s">
+        <v>258</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>"Entrou em Contato para Alterar Plano"</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["E3"] ="Entrou em Contato para Alterar Plano"</v>
+      </c>
+      <c r="E38" t="s">
+        <v>260</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Entrou em Contato para Alterar Plano", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G38" t="s">
+        <v>261</v>
+      </c>
+      <c r="I38" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>232</v>
+      </c>
+      <c r="B39" t="s">
+        <v>258</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT Resolução Alteração"</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["E4"] ="SAT Resolução Alteração"</v>
+      </c>
+      <c r="E39" t="s">
+        <v>260</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT Resolução Alteração", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G39" t="s">
+        <v>261</v>
+      </c>
+      <c r="I39" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>233</v>
+      </c>
+      <c r="B40" t="s">
+        <v>258</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>"Entrou em Contato para Cancelar"</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["E5"] ="Entrou em Contato para Cancelar"</v>
+      </c>
+      <c r="E40" t="s">
+        <v>260</v>
+      </c>
+      <c r="F40" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Entrou em Contato para Cancelar", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G40" t="s">
+        <v>261</v>
+      </c>
+      <c r="I40" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>234</v>
+      </c>
+      <c r="B41" t="s">
+        <v>258</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT Resolução Cancelamento"</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["E6"] ="SAT Resolução Cancelamento"</v>
+      </c>
+      <c r="E41" t="s">
+        <v>260</v>
+      </c>
+      <c r="F41" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT Resolução Cancelamento", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G41" t="s">
+        <v>261</v>
+      </c>
+      <c r="I41" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>235</v>
+      </c>
+      <c r="B42" t="s">
+        <v>258</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>"Entrou em Contato para Problemas"</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["E7"] ="Entrou em Contato para Problemas"</v>
+      </c>
+      <c r="E42" t="s">
+        <v>260</v>
+      </c>
+      <c r="F42" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Entrou em Contato para Problemas", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G42" t="s">
+        <v>261</v>
+      </c>
+      <c r="I42" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>236</v>
+      </c>
+      <c r="B43" t="s">
+        <v>258</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT a resolução do Problema"</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["E8"] ="SAT a resolução do Problema"</v>
+      </c>
+      <c r="E43" t="s">
+        <v>260</v>
+      </c>
+      <c r="F43" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT a resolução do Problema", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G43" t="s">
+        <v>261</v>
+      </c>
+      <c r="I43" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>237</v>
+      </c>
+      <c r="B44" t="s">
+        <v>258</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>"Solicitou instalação de internet fixa"</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["F1"] ="Solicitou instalação de internet fixa"</v>
+      </c>
+      <c r="E44" t="s">
+        <v>260</v>
+      </c>
+      <c r="F44" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Solicitou instalação de internet fixa", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G44" t="s">
+        <v>261</v>
+      </c>
+      <c r="I44" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>238</v>
+      </c>
+      <c r="B45" t="s">
+        <v>258</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT Solicitação de Instalação"</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["F2_1"] ="SAT Solicitação de Instalação"</v>
+      </c>
+      <c r="E45" t="s">
+        <v>260</v>
+      </c>
+      <c r="F45" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT Solicitação de Instalação", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G45" t="s">
+        <v>261</v>
+      </c>
+      <c r="I45" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>239</v>
+      </c>
+      <c r="B46" t="s">
+        <v>258</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT Prazo Instalação"</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["F2_2"] ="SAT Prazo Instalação"</v>
+      </c>
+      <c r="E46" t="s">
+        <v>260</v>
+      </c>
+      <c r="F46" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT Prazo Instalação", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G46" t="s">
+        <v>261</v>
+      </c>
+      <c r="I46" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>240</v>
+      </c>
+      <c r="B47" t="s">
+        <v>258</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT Qualidade Instalação"</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["F2_3"] ="SAT Qualidade Instalação"</v>
+      </c>
+      <c r="E47" t="s">
+        <v>260</v>
+      </c>
+      <c r="F47" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT Qualidade Instalação", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G47" t="s">
+        <v>261</v>
+      </c>
+      <c r="I47" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>241</v>
+      </c>
+      <c r="B48" t="s">
+        <v>258</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>"Solicito reparos"</v>
+      </c>
+      <c r="D48" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["F3"] ="Solicito reparos"</v>
+      </c>
+      <c r="E48" t="s">
+        <v>260</v>
+      </c>
+      <c r="F48" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Solicito reparos", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G48" t="s">
+        <v>261</v>
+      </c>
+      <c r="I48" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>242</v>
+      </c>
+      <c r="B49" t="s">
+        <v>258</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT Reparos"</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["F4_1"] ="SAT Reparos"</v>
+      </c>
+      <c r="E49" t="s">
+        <v>260</v>
+      </c>
+      <c r="F49" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT Reparos", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G49" t="s">
+        <v>261</v>
+      </c>
+      <c r="I49" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>243</v>
+      </c>
+      <c r="B50" t="s">
+        <v>258</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT Prazo Reparos"</v>
+      </c>
+      <c r="D50" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["F4_2"] ="SAT Prazo Reparos"</v>
+      </c>
+      <c r="E50" t="s">
+        <v>260</v>
+      </c>
+      <c r="F50" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT Prazo Reparos", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G50" t="s">
+        <v>261</v>
+      </c>
+      <c r="I50" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>244</v>
+      </c>
+      <c r="B51" t="s">
+        <v>258</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>"SAT Qualidade Reparos"</v>
+      </c>
+      <c r="D51" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["F4_3"] ="SAT Qualidade Reparos"</v>
+      </c>
+      <c r="E51" t="s">
+        <v>260</v>
+      </c>
+      <c r="F51" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("SAT Qualidade Reparos", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G51" t="s">
+        <v>261</v>
+      </c>
+      <c r="I51" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>245</v>
+      </c>
+      <c r="B52" t="s">
+        <v>258</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>"Existência de Outra Operadora"</v>
+      </c>
+      <c r="D52" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["G1"] ="Existência de Outra Operadora"</v>
+      </c>
+      <c r="E52" t="s">
+        <v>260</v>
+      </c>
+      <c r="F52" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Existência de Outra Operadora", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G52" t="s">
+        <v>261</v>
+      </c>
+      <c r="I52" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>246</v>
+      </c>
+      <c r="B53" t="s">
+        <v>258</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>"Inclui TV?"</v>
+      </c>
+      <c r="D53" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["G2_1"] ="Inclui TV?"</v>
+      </c>
+      <c r="E53" t="s">
+        <v>260</v>
+      </c>
+      <c r="F53" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Inclui TV?", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G53" t="s">
+        <v>261</v>
+      </c>
+      <c r="I53" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>247</v>
+      </c>
+      <c r="B54" t="s">
+        <v>258</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>"Inclui Telefonia Móvel?"</v>
+      </c>
+      <c r="D54" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["G2_2"] ="Inclui Telefonia Móvel?"</v>
+      </c>
+      <c r="E54" t="s">
+        <v>260</v>
+      </c>
+      <c r="F54" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Inclui Telefonia Móvel?", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G54" t="s">
+        <v>261</v>
+      </c>
+      <c r="I54" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>248</v>
+      </c>
+      <c r="B55" t="s">
+        <v>258</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>"Inclui Telefone Fixo"</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["G2_3"] ="Inclui Telefone Fixo"</v>
+      </c>
+      <c r="E55" t="s">
+        <v>260</v>
+      </c>
+      <c r="F55" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Inclui Telefone Fixo", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G55" t="s">
+        <v>261</v>
+      </c>
+      <c r="I55" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>249</v>
+      </c>
+      <c r="B56" t="s">
+        <v>258</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>"Município"</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["H0"] ="Município"</v>
+      </c>
+      <c r="E56" t="s">
+        <v>260</v>
+      </c>
+      <c r="F56" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Município", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G56" t="s">
+        <v>261</v>
+      </c>
+      <c r="I56" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>250</v>
+      </c>
+      <c r="B57" t="s">
+        <v>258</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v>"IBGE"</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["H1"] ="IBGE"</v>
+      </c>
+      <c r="E57" t="s">
+        <v>260</v>
+      </c>
+      <c r="F57" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("IBGE", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G57" t="s">
+        <v>261</v>
+      </c>
+      <c r="I57" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>251</v>
+      </c>
+      <c r="B58" t="s">
+        <v>258</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>"Quantidade de pessoas"</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["H2"] ="Quantidade de pessoas"</v>
+      </c>
+      <c r="E58" t="s">
+        <v>260</v>
+      </c>
+      <c r="F58" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Quantidade de pessoas", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G58" t="s">
+        <v>261</v>
+      </c>
+      <c r="I58" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>252</v>
+      </c>
+      <c r="B59" t="s">
+        <v>258</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>"Renda"</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["H2a"] ="Renda"</v>
+      </c>
+      <c r="E59" t="s">
+        <v>260</v>
+      </c>
+      <c r="F59" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Renda", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G59" t="s">
+        <v>261</v>
+      </c>
+      <c r="I59" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>253</v>
+      </c>
+      <c r="B60" t="s">
+        <v>258</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v>"Recusa Renda"</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["H3"] ="Recusa Renda"</v>
+      </c>
+      <c r="E60" t="s">
+        <v>260</v>
+      </c>
+      <c r="F60" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Recusa Renda", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G60" t="s">
+        <v>261</v>
+      </c>
+      <c r="I60" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>254</v>
+      </c>
+      <c r="B61" t="s">
+        <v>258</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v>"H3"</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["I1"] ="H3"</v>
+      </c>
+      <c r="E61" t="s">
+        <v>260</v>
+      </c>
+      <c r="F61" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("H3", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G61" t="s">
+        <v>261</v>
+      </c>
+      <c r="I61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>255</v>
+      </c>
+      <c r="B62" t="s">
+        <v>258</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v>"Autorização 1"</v>
+      </c>
+      <c r="D62" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["I2"] ="Autorização 1"</v>
+      </c>
+      <c r="E62" t="s">
+        <v>260</v>
+      </c>
+      <c r="F62" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Autorização 1", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G62" t="s">
+        <v>261</v>
+      </c>
+      <c r="I62" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>256</v>
+      </c>
+      <c r="B63" t="s">
+        <v>258</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v>"Autorização 2"</v>
+      </c>
+      <c r="D63" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["PESO"] ="Autorização 2"</v>
+      </c>
+      <c r="E63" t="s">
+        <v>260</v>
+      </c>
+      <c r="F63" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("Autorização 2", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G63" t="s">
+        <v>261</v>
+      </c>
+      <c r="I63" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>257</v>
+      </c>
+      <c r="B64" t="s">
+        <v>258</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v>"PESO"</v>
+      </c>
+      <c r="D64" t="str">
+        <f t="shared" si="1"/>
+        <v>Glossario["COD_IBGE"] ="PESO"</v>
+      </c>
+      <c r="E64" t="s">
+        <v>260</v>
+      </c>
+      <c r="F64" t="str">
+        <f t="shared" si="2"/>
+        <v>Data_Reshaped.drop("PESO", inplace= True, axis = 1)</v>
+      </c>
+      <c r="G64" t="s">
+        <v>261</v>
+      </c>
+      <c r="I64" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:I64"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>